<commit_message>
arbeitsjournale angepasst nik fer
</commit_message>
<xml_diff>
--- a/Arbeitsjournale/2Semester/Arbeitsjournal Fernando.xlsx
+++ b/Arbeitsjournale/2Semester/Arbeitsjournal Fernando.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22340" windowHeight="15840"/>
+    <workbookView xWindow="10640" yWindow="500" windowWidth="22340" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Arbeitsjournal Semesterarbeit</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>Name: Fernando Maniglio</t>
+  </si>
+  <si>
+    <t>View für Logging erstellt</t>
+  </si>
+  <si>
+    <t>privileges angefangen mit nik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privileges fertiggestellt </t>
+  </si>
+  <si>
+    <t>Doku</t>
   </si>
 </sst>
 </file>
@@ -501,7 +513,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -765,9 +777,15 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="11">
+        <v>43532</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -793,9 +811,15 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="11">
+        <v>43532</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -821,9 +845,15 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="11">
+        <v>43533</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -849,9 +879,15 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="11">
+        <v>43534</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1583,7 +1619,7 @@
       <c r="B38" s="18"/>
       <c r="C38" s="19">
         <f>SUM(C6:C36)</f>
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>

</xml_diff>